<commit_message>
Changed locator and worked on author
</commit_message>
<xml_diff>
--- a/testData/authorTestTabTestData/authorTestCaseTab_testData.xlsx
+++ b/testData/authorTestTabTestData/authorTestCaseTab_testData.xlsx
@@ -1,72 +1,67 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29127"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3B48B7B9-66BA-45E3-AB82-9A8FF6DBF20F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MohitAman\Desktop\UAT_NEXTNEXT_BLAZE_FRAMEWORK_AUTO\testData\authorTestTabTestData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BE75CED-341C-4F3F-8A1F-1DCDBE15E11F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6800" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddTest" sheetId="2" r:id="rId1"/>
     <sheet name="tc001" sheetId="3" r:id="rId2"/>
     <sheet name="tc003" sheetId="1" r:id="rId3"/>
-    <sheet name="tc004" sheetId="4" r:id="rId4"/>
-    <sheet name="tc007" sheetId="5" r:id="rId5"/>
-    <sheet name="tc009" sheetId="6" r:id="rId6"/>
-    <sheet name="tc011" sheetId="7" r:id="rId7"/>
-    <sheet name="tc018" sheetId="8" r:id="rId8"/>
-    <sheet name="tc028" sheetId="9" r:id="rId9"/>
-    <sheet name="tc029" sheetId="10" r:id="rId10"/>
-    <sheet name="tc034" sheetId="11" r:id="rId11"/>
-    <sheet name="tc035" sheetId="13" r:id="rId12"/>
-    <sheet name="tc039" sheetId="15" r:id="rId13"/>
-    <sheet name="tc040" sheetId="14" r:id="rId14"/>
-    <sheet name="tc042" sheetId="28" r:id="rId15"/>
-    <sheet name="tc044" sheetId="29" r:id="rId16"/>
-    <sheet name="tc045" sheetId="17" r:id="rId17"/>
-    <sheet name="tc046" sheetId="18" r:id="rId18"/>
-    <sheet name="tc047" sheetId="16" r:id="rId19"/>
-    <sheet name="tc049" sheetId="24" r:id="rId20"/>
-    <sheet name="tc053" sheetId="19" r:id="rId21"/>
-    <sheet name="tc056" sheetId="21" r:id="rId22"/>
-    <sheet name="tc057" sheetId="22" r:id="rId23"/>
-    <sheet name="tc058" sheetId="20" r:id="rId24"/>
-    <sheet name="tc063" sheetId="23" r:id="rId25"/>
-    <sheet name="tc070" sheetId="25" r:id="rId26"/>
-    <sheet name="tc071" sheetId="26" r:id="rId27"/>
-    <sheet name="tc072" sheetId="27" r:id="rId28"/>
-    <sheet name="tc073" sheetId="30" r:id="rId29"/>
-    <sheet name="tc041" sheetId="31" r:id="rId30"/>
-    <sheet name="tc051" sheetId="32" r:id="rId31"/>
-    <sheet name="tc052" sheetId="33" r:id="rId32"/>
-    <sheet name="tc059" sheetId="34" r:id="rId33"/>
-    <sheet name="tc066" sheetId="35" r:id="rId34"/>
-    <sheet name="tc067" sheetId="36" r:id="rId35"/>
-    <sheet name="tc060" sheetId="37" r:id="rId36"/>
+    <sheet name="tc036" sheetId="38" r:id="rId4"/>
+    <sheet name="tc004" sheetId="4" r:id="rId5"/>
+    <sheet name="tc007" sheetId="5" r:id="rId6"/>
+    <sheet name="tc009" sheetId="6" r:id="rId7"/>
+    <sheet name="tc011" sheetId="7" r:id="rId8"/>
+    <sheet name="tc018" sheetId="8" r:id="rId9"/>
+    <sheet name="tc028" sheetId="9" r:id="rId10"/>
+    <sheet name="tc029" sheetId="10" r:id="rId11"/>
+    <sheet name="tc034" sheetId="11" r:id="rId12"/>
+    <sheet name="tc035" sheetId="13" r:id="rId13"/>
+    <sheet name="tc039" sheetId="15" r:id="rId14"/>
+    <sheet name="tc040" sheetId="14" r:id="rId15"/>
+    <sheet name="tc042" sheetId="28" r:id="rId16"/>
+    <sheet name="tc044" sheetId="29" r:id="rId17"/>
+    <sheet name="tc045" sheetId="17" r:id="rId18"/>
+    <sheet name="tc046" sheetId="18" r:id="rId19"/>
+    <sheet name="tc047" sheetId="16" r:id="rId20"/>
+    <sheet name="tc049" sheetId="24" r:id="rId21"/>
+    <sheet name="tc053" sheetId="19" r:id="rId22"/>
+    <sheet name="tc056" sheetId="21" r:id="rId23"/>
+    <sheet name="tc057" sheetId="22" r:id="rId24"/>
+    <sheet name="tc058" sheetId="20" r:id="rId25"/>
+    <sheet name="tc063" sheetId="23" r:id="rId26"/>
+    <sheet name="tc070" sheetId="25" r:id="rId27"/>
+    <sheet name="tc071" sheetId="26" r:id="rId28"/>
+    <sheet name="tc072" sheetId="27" r:id="rId29"/>
+    <sheet name="tc073" sheetId="30" r:id="rId30"/>
+    <sheet name="tc041" sheetId="31" r:id="rId31"/>
+    <sheet name="tc051" sheetId="32" r:id="rId32"/>
+    <sheet name="tc052" sheetId="33" r:id="rId33"/>
+    <sheet name="tc059" sheetId="34" r:id="rId34"/>
+    <sheet name="tc066" sheetId="35" r:id="rId35"/>
+    <sheet name="tc067" sheetId="36" r:id="rId36"/>
+    <sheet name="tc060" sheetId="37" r:id="rId37"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="68">
   <si>
     <t>Epic</t>
   </si>
@@ -74,40 +69,16 @@
     <t>Feature</t>
   </si>
   <si>
-    <t>RequirementId</t>
-  </si>
-  <si>
-    <t>TestCaseName</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
     <t>Priority</t>
   </si>
   <si>
-    <t>QA</t>
-  </si>
-  <si>
     <t>Epic Mohit</t>
   </si>
   <si>
     <t>Feature Mohit</t>
   </si>
   <si>
-    <t>RQ-679</t>
-  </si>
-  <si>
-    <t>Tc-08</t>
-  </si>
-  <si>
-    <t>As a tester I want to test so that..</t>
-  </si>
-  <si>
     <t>Low</t>
-  </si>
-  <si>
-    <t>Mayukhjit Chakraborty</t>
   </si>
   <si>
     <t>Label Name</t>
@@ -300,7 +271,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -331,12 +302,6 @@
       <name val="Aptos Narrow"/>
       <charset val="134"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF0BA5EC"/>
-      <name val="Arial"/>
-      <charset val="1"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -358,7 +323,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -367,7 +332,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -643,58 +607,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.45"/>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" t="s">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:G1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="29">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="29">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="14.25">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
+      <c r="B2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -703,6 +643,29 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -710,11 +673,11 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:1">
@@ -727,151 +690,151 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.45"/>
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="17.875" customWidth="1"/>
-    <col min="3" max="3" width="18.25" customWidth="1"/>
+    <col min="2" max="2" width="17.90625" customWidth="1"/>
+    <col min="3" max="3" width="18.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="14.90625" customWidth="1"/>
+    <col min="2" max="2" width="13.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="29">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="D2" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
       <c r="B1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>7</v>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>22</v>
       </c>
       <c r="B2" t="s">
         <v>28</v>
       </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.45"/>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>30</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.45"/>
-  <cols>
-    <col min="1" max="1" width="14.875" customWidth="1"/>
-    <col min="2" max="2" width="13.875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="29.1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.45"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{086FC864-88BE-4524-8C8E-D67D5CC31D33}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -879,34 +842,34 @@
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="14.125" customWidth="1"/>
+    <col min="5" max="5" width="14.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8253E48-AC13-4C68-9E15-DF10E463748C}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -914,27 +877,27 @@
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="3" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -942,9 +905,9 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.45"/>
-  <sheetData>
-    <row r="1" spans="1:4" ht="29.1">
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:4" ht="29">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -952,24 +915,24 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="29.1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="29">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -977,7 +940,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -985,9 +948,9 @@
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.45"/>
-  <sheetData>
-    <row r="1" spans="1:5" ht="29.1">
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="29">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -995,55 +958,30 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="29.1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="29">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.45"/>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1057,11 +995,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="10.7265625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:1">
@@ -1075,6 +1016,31 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5C16204-518F-4A99-9E15-92D9161822C5}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1082,30 +1048,30 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1113,10 +1079,10 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="19.875" customWidth="1"/>
-    <col min="3" max="3" width="10.25" customWidth="1"/>
+    <col min="2" max="2" width="19.90625" customWidth="1"/>
+    <col min="3" max="3" width="10.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1127,21 +1093,21 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -1152,13 +1118,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16CA93A4-EF19-4F56-9442-DB07645E3971}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
@@ -1168,85 +1134,85 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E1" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3C6F736-6B6A-4D47-9A3D-6735D564D2A8}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
         <v>33</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
       </c>
       <c r="D2" t="s">
         <v>34</v>
       </c>
       <c r="E2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3C6F736-6B6A-4D47-9A3D-6735D564D2A8}">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -1254,39 +1220,39 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="13.5" customWidth="1"/>
-    <col min="4" max="4" width="13.125" customWidth="1"/>
-    <col min="6" max="6" width="19.875" customWidth="1"/>
+    <col min="2" max="2" width="13.453125" customWidth="1"/>
+    <col min="4" max="4" width="13.08984375" customWidth="1"/>
+    <col min="6" max="6" width="19.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" t="s">
         <v>48</v>
       </c>
-      <c r="B1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E1" t="s">
-        <v>56</v>
-      </c>
       <c r="F1" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C2">
         <v>5</v>
@@ -1306,7 +1272,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{279E3CF8-6B58-482B-86D6-D534C8F178AB}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1314,34 +1280,34 @@
       <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="12.875" customWidth="1"/>
-    <col min="2" max="2" width="14.375" customWidth="1"/>
+    <col min="1" max="1" width="12.90625" customWidth="1"/>
+    <col min="2" max="2" width="14.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FBC1A4B-7999-43EC-A9B0-80154C608585}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1349,27 +1315,27 @@
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="22.75" customWidth="1"/>
+    <col min="1" max="1" width="22.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1904BE75-2DA2-4667-82ED-527A58FD3287}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1377,27 +1343,27 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="16.25" customWidth="1"/>
+    <col min="1" max="1" width="16.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EBEBA48-046F-4F91-8E90-E6AC9BDD1146}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1405,79 +1371,25 @@
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="14.625" customWidth="1"/>
+    <col min="1" max="1" width="14.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F856F1BD-60DF-4B45-AA48-6580610D0108}">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
-  <cols>
-    <col min="1" max="1" width="13.75" customWidth="1"/>
-    <col min="2" max="2" width="17.375" customWidth="1"/>
-    <col min="3" max="3" width="15.25" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="33">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="33">
-      <c r="A2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1489,195 +1401,195 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.45"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="30.5" customWidth="1"/>
+    <col min="1" max="1" width="30.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="13.5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15">
       <c r="A2" s="5" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B20" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B21" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B22" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1686,6 +1598,60 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F856F1BD-60DF-4B45-AA48-6580610D0108}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="13.7265625" customWidth="1"/>
+    <col min="2" max="2" width="17.36328125" customWidth="1"/>
+    <col min="3" max="3" width="15.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A2AE599-8749-4FEB-AADF-97800FD166F6}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -1693,65 +1659,65 @@
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="3" max="3" width="9.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" t="s">
         <v>63</v>
       </c>
-      <c r="B1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="G2" t="s">
         <v>64</v>
       </c>
-      <c r="D1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC885B18-8D7B-4141-98D3-4064592E6866}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -1759,63 +1725,63 @@
       <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="6" max="6" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" t="s">
         <v>63</v>
       </c>
-      <c r="B1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="G2" t="s">
         <v>64</v>
       </c>
-      <c r="D1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B4F42AD-06FB-4F9A-BDC5-0D988CFBC7C0}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1823,30 +1789,30 @@
       <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B1" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DD0E29D-0CA1-467B-B75D-731ABD724820}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1854,30 +1820,30 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B1" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32378A89-E73B-434C-9031-5BC597A1049F}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1885,24 +1851,24 @@
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
-  <sheetData>
-    <row r="1" spans="1:1" ht="14.25">
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:1">
       <c r="A1" s="4" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01634569-4DCA-4114-8B9F-D11F9C8D6829}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1910,45 +1876,45 @@
       <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
-  <sheetData>
-    <row r="1" spans="1:1" ht="14.25">
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:1">
       <c r="A1" s="4" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32EC422E-61E5-4D5C-9000-57CFDB7C1C6E}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B1" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1957,6 +1923,48 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9A9333D-303C-4846-B6A8-32400E420636}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="14.26953125" customWidth="1"/>
+    <col min="2" max="2" width="13.26953125" customWidth="1"/>
+    <col min="3" max="3" width="14.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="17" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="17.5" customHeight="1">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1964,7 +1972,7 @@
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
@@ -1973,25 +1981,25 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -1999,24 +2007,24 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
@@ -2025,21 +2033,21 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -2051,68 +2059,45 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.45"/>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes done in TC48 data and added wait
</commit_message>
<xml_diff>
--- a/testData/authorTestTabTestData/authorTestCaseTab_testData.xlsx
+++ b/testData/authorTestTabTestData/authorTestCaseTab_testData.xlsx
@@ -8,48 +8,49 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MohitAman\Desktop\UAT_NEXTNEXT_BLAZE_FRAMEWORK_AUTO\testData\authorTestTabTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C98232C8-4075-43E1-AE86-8457803D6075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5094D386-609D-4B9D-AA74-C32B65D6B7B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddTest" sheetId="2" r:id="rId1"/>
-    <sheet name="tc001" sheetId="3" r:id="rId2"/>
-    <sheet name="tc003" sheetId="1" r:id="rId3"/>
-    <sheet name="tc036" sheetId="38" r:id="rId4"/>
-    <sheet name="tc004" sheetId="4" r:id="rId5"/>
-    <sheet name="tc007" sheetId="5" r:id="rId6"/>
-    <sheet name="tc009" sheetId="6" r:id="rId7"/>
-    <sheet name="tc011" sheetId="7" r:id="rId8"/>
-    <sheet name="tc018" sheetId="8" r:id="rId9"/>
-    <sheet name="tc028" sheetId="9" r:id="rId10"/>
-    <sheet name="tc029" sheetId="10" r:id="rId11"/>
-    <sheet name="tc034" sheetId="11" r:id="rId12"/>
-    <sheet name="tc035" sheetId="13" r:id="rId13"/>
-    <sheet name="tc039" sheetId="15" r:id="rId14"/>
-    <sheet name="tc040" sheetId="14" r:id="rId15"/>
-    <sheet name="tc042" sheetId="28" r:id="rId16"/>
-    <sheet name="tc044" sheetId="29" r:id="rId17"/>
-    <sheet name="tc045" sheetId="17" r:id="rId18"/>
-    <sheet name="tc046" sheetId="18" r:id="rId19"/>
-    <sheet name="tc047" sheetId="16" r:id="rId20"/>
-    <sheet name="tc049" sheetId="24" r:id="rId21"/>
-    <sheet name="tc053" sheetId="19" r:id="rId22"/>
-    <sheet name="tc056" sheetId="21" r:id="rId23"/>
-    <sheet name="tc057" sheetId="22" r:id="rId24"/>
-    <sheet name="tc058" sheetId="20" r:id="rId25"/>
-    <sheet name="tc063" sheetId="23" r:id="rId26"/>
-    <sheet name="tc070" sheetId="25" r:id="rId27"/>
-    <sheet name="tc071" sheetId="26" r:id="rId28"/>
-    <sheet name="tc072" sheetId="27" r:id="rId29"/>
-    <sheet name="tc073" sheetId="30" r:id="rId30"/>
-    <sheet name="tc041" sheetId="31" r:id="rId31"/>
-    <sheet name="tc051" sheetId="32" r:id="rId32"/>
-    <sheet name="tc052" sheetId="33" r:id="rId33"/>
-    <sheet name="tc059" sheetId="34" r:id="rId34"/>
-    <sheet name="tc066" sheetId="35" r:id="rId35"/>
-    <sheet name="tc067" sheetId="36" r:id="rId36"/>
-    <sheet name="tc060" sheetId="37" r:id="rId37"/>
+    <sheet name="tc048" sheetId="39" r:id="rId2"/>
+    <sheet name="tc001" sheetId="3" r:id="rId3"/>
+    <sheet name="tc003" sheetId="1" r:id="rId4"/>
+    <sheet name="tc036" sheetId="38" r:id="rId5"/>
+    <sheet name="tc004" sheetId="4" r:id="rId6"/>
+    <sheet name="tc007" sheetId="5" r:id="rId7"/>
+    <sheet name="tc009" sheetId="6" r:id="rId8"/>
+    <sheet name="tc011" sheetId="7" r:id="rId9"/>
+    <sheet name="tc018" sheetId="8" r:id="rId10"/>
+    <sheet name="tc028" sheetId="9" r:id="rId11"/>
+    <sheet name="tc029" sheetId="10" r:id="rId12"/>
+    <sheet name="tc034" sheetId="11" r:id="rId13"/>
+    <sheet name="tc035" sheetId="13" r:id="rId14"/>
+    <sheet name="tc039" sheetId="15" r:id="rId15"/>
+    <sheet name="tc040" sheetId="14" r:id="rId16"/>
+    <sheet name="tc042" sheetId="28" r:id="rId17"/>
+    <sheet name="tc044" sheetId="29" r:id="rId18"/>
+    <sheet name="tc045" sheetId="17" r:id="rId19"/>
+    <sheet name="tc046" sheetId="18" r:id="rId20"/>
+    <sheet name="tc047" sheetId="16" r:id="rId21"/>
+    <sheet name="tc049" sheetId="24" r:id="rId22"/>
+    <sheet name="tc053" sheetId="19" r:id="rId23"/>
+    <sheet name="tc056" sheetId="21" r:id="rId24"/>
+    <sheet name="tc057" sheetId="22" r:id="rId25"/>
+    <sheet name="tc058" sheetId="20" r:id="rId26"/>
+    <sheet name="tc063" sheetId="23" r:id="rId27"/>
+    <sheet name="tc070" sheetId="25" r:id="rId28"/>
+    <sheet name="tc071" sheetId="26" r:id="rId29"/>
+    <sheet name="tc072" sheetId="27" r:id="rId30"/>
+    <sheet name="tc073" sheetId="30" r:id="rId31"/>
+    <sheet name="tc041" sheetId="31" r:id="rId32"/>
+    <sheet name="tc051" sheetId="32" r:id="rId33"/>
+    <sheet name="tc052" sheetId="33" r:id="rId34"/>
+    <sheet name="tc059" sheetId="34" r:id="rId35"/>
+    <sheet name="tc066" sheetId="35" r:id="rId36"/>
+    <sheet name="tc067" sheetId="36" r:id="rId37"/>
+    <sheet name="tc060" sheetId="37" r:id="rId38"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -61,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="73">
   <si>
     <t>Epic</t>
   </si>
@@ -265,6 +266,21 @@
   </si>
   <si>
     <t>tcId</t>
+  </si>
+  <si>
+    <t>Tcname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit testing </t>
+  </si>
+  <si>
+    <t>Tcdescription</t>
+  </si>
+  <si>
+    <t>work</t>
+  </si>
+  <si>
+    <t>QA</t>
   </si>
 </sst>
 </file>
@@ -609,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -643,6 +659,41 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -665,7 +716,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -690,7 +741,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -731,7 +782,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -756,7 +807,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -803,7 +854,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -834,7 +885,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{086FC864-88BE-4524-8C8E-D67D5CC31D33}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -869,7 +920,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8253E48-AC13-4C68-9E15-DF10E463748C}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -897,7 +948,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -940,7 +991,68 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDAB02CB-AF8A-49D3-8080-6FFA51EF7AC4}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="29">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="29">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -989,33 +1101,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="10.7265625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1040,7 +1126,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5C16204-518F-4A99-9E15-92D9161822C5}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1071,7 +1157,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1118,7 +1204,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16CA93A4-EF19-4F56-9442-DB07645E3971}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1165,7 +1251,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3C6F736-6B6A-4D47-9A3D-6735D564D2A8}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1212,7 +1298,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -1272,7 +1358,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{279E3CF8-6B58-482B-86D6-D534C8F178AB}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1307,7 +1393,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FBC1A4B-7999-43EC-A9B0-80154C608585}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1335,7 +1421,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1904BE75-2DA2-4667-82ED-527A58FD3287}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1363,7 +1449,33 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="10.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EBEBA48-046F-4F91-8E90-E6AC9BDD1146}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1397,207 +1509,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D22"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="30.453125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15">
-      <c r="A2" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
-        <v>9</v>
-      </c>
-      <c r="B20" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F856F1BD-60DF-4B45-AA48-6580610D0108}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1651,7 +1563,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A2AE599-8749-4FEB-AADF-97800FD166F6}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -1717,7 +1629,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC885B18-8D7B-4141-98D3-4064592E6866}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -1781,7 +1693,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B4F42AD-06FB-4F9A-BDC5-0D988CFBC7C0}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1812,7 +1724,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DD0E29D-0CA1-467B-B75D-731ABD724820}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1843,7 +1755,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32378A89-E73B-434C-9031-5BC597A1049F}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1868,7 +1780,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01634569-4DCA-4114-8B9F-D11F9C8D6829}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1893,7 +1805,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32EC422E-61E5-4D5C-9000-57CFDB7C1C6E}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1923,6 +1835,206 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="30.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15">
+      <c r="A2" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9A9333D-303C-4846-B6A8-32400E420636}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -1964,7 +2076,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1989,7 +2101,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -2018,7 +2130,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -2041,7 +2153,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -2068,39 +2180,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
changes done in TC37 data and added wait
</commit_message>
<xml_diff>
--- a/testData/authorTestTabTestData/authorTestCaseTab_testData.xlsx
+++ b/testData/authorTestTabTestData/authorTestCaseTab_testData.xlsx
@@ -8,49 +8,50 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MohitAman\Desktop\UAT_NEXTNEXT_BLAZE_FRAMEWORK_AUTO\testData\authorTestTabTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5094D386-609D-4B9D-AA74-C32B65D6B7B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD798677-95C6-4308-B415-C91F71D511B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddTest" sheetId="2" r:id="rId1"/>
     <sheet name="tc048" sheetId="39" r:id="rId2"/>
-    <sheet name="tc001" sheetId="3" r:id="rId3"/>
-    <sheet name="tc003" sheetId="1" r:id="rId4"/>
-    <sheet name="tc036" sheetId="38" r:id="rId5"/>
-    <sheet name="tc004" sheetId="4" r:id="rId6"/>
-    <sheet name="tc007" sheetId="5" r:id="rId7"/>
-    <sheet name="tc009" sheetId="6" r:id="rId8"/>
-    <sheet name="tc011" sheetId="7" r:id="rId9"/>
-    <sheet name="tc018" sheetId="8" r:id="rId10"/>
-    <sheet name="tc028" sheetId="9" r:id="rId11"/>
-    <sheet name="tc029" sheetId="10" r:id="rId12"/>
-    <sheet name="tc034" sheetId="11" r:id="rId13"/>
-    <sheet name="tc035" sheetId="13" r:id="rId14"/>
-    <sheet name="tc039" sheetId="15" r:id="rId15"/>
-    <sheet name="tc040" sheetId="14" r:id="rId16"/>
-    <sheet name="tc042" sheetId="28" r:id="rId17"/>
-    <sheet name="tc044" sheetId="29" r:id="rId18"/>
-    <sheet name="tc045" sheetId="17" r:id="rId19"/>
-    <sheet name="tc046" sheetId="18" r:id="rId20"/>
-    <sheet name="tc047" sheetId="16" r:id="rId21"/>
-    <sheet name="tc049" sheetId="24" r:id="rId22"/>
-    <sheet name="tc053" sheetId="19" r:id="rId23"/>
-    <sheet name="tc056" sheetId="21" r:id="rId24"/>
-    <sheet name="tc057" sheetId="22" r:id="rId25"/>
-    <sheet name="tc058" sheetId="20" r:id="rId26"/>
-    <sheet name="tc063" sheetId="23" r:id="rId27"/>
-    <sheet name="tc070" sheetId="25" r:id="rId28"/>
-    <sheet name="tc071" sheetId="26" r:id="rId29"/>
-    <sheet name="tc072" sheetId="27" r:id="rId30"/>
-    <sheet name="tc073" sheetId="30" r:id="rId31"/>
-    <sheet name="tc041" sheetId="31" r:id="rId32"/>
-    <sheet name="tc051" sheetId="32" r:id="rId33"/>
-    <sheet name="tc052" sheetId="33" r:id="rId34"/>
-    <sheet name="tc059" sheetId="34" r:id="rId35"/>
-    <sheet name="tc066" sheetId="35" r:id="rId36"/>
-    <sheet name="tc067" sheetId="36" r:id="rId37"/>
-    <sheet name="tc060" sheetId="37" r:id="rId38"/>
+    <sheet name="tc037" sheetId="40" r:id="rId3"/>
+    <sheet name="tc001" sheetId="3" r:id="rId4"/>
+    <sheet name="tc003" sheetId="1" r:id="rId5"/>
+    <sheet name="tc036" sheetId="38" r:id="rId6"/>
+    <sheet name="tc004" sheetId="4" r:id="rId7"/>
+    <sheet name="tc007" sheetId="5" r:id="rId8"/>
+    <sheet name="tc009" sheetId="6" r:id="rId9"/>
+    <sheet name="tc011" sheetId="7" r:id="rId10"/>
+    <sheet name="tc018" sheetId="8" r:id="rId11"/>
+    <sheet name="tc028" sheetId="9" r:id="rId12"/>
+    <sheet name="tc029" sheetId="10" r:id="rId13"/>
+    <sheet name="tc034" sheetId="11" r:id="rId14"/>
+    <sheet name="tc035" sheetId="13" r:id="rId15"/>
+    <sheet name="tc039" sheetId="15" r:id="rId16"/>
+    <sheet name="tc040" sheetId="14" r:id="rId17"/>
+    <sheet name="tc042" sheetId="28" r:id="rId18"/>
+    <sheet name="tc044" sheetId="29" r:id="rId19"/>
+    <sheet name="tc045" sheetId="17" r:id="rId20"/>
+    <sheet name="tc046" sheetId="18" r:id="rId21"/>
+    <sheet name="tc047" sheetId="16" r:id="rId22"/>
+    <sheet name="tc049" sheetId="24" r:id="rId23"/>
+    <sheet name="tc053" sheetId="19" r:id="rId24"/>
+    <sheet name="tc056" sheetId="21" r:id="rId25"/>
+    <sheet name="tc057" sheetId="22" r:id="rId26"/>
+    <sheet name="tc058" sheetId="20" r:id="rId27"/>
+    <sheet name="tc063" sheetId="23" r:id="rId28"/>
+    <sheet name="tc070" sheetId="25" r:id="rId29"/>
+    <sheet name="tc071" sheetId="26" r:id="rId30"/>
+    <sheet name="tc072" sheetId="27" r:id="rId31"/>
+    <sheet name="tc073" sheetId="30" r:id="rId32"/>
+    <sheet name="tc041" sheetId="31" r:id="rId33"/>
+    <sheet name="tc051" sheetId="32" r:id="rId34"/>
+    <sheet name="tc052" sheetId="33" r:id="rId35"/>
+    <sheet name="tc059" sheetId="34" r:id="rId36"/>
+    <sheet name="tc066" sheetId="35" r:id="rId37"/>
+    <sheet name="tc067" sheetId="36" r:id="rId38"/>
+    <sheet name="tc060" sheetId="37" r:id="rId39"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="73">
   <si>
     <t>Epic</t>
   </si>
@@ -659,6 +660,35 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -693,7 +723,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -716,7 +746,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -741,7 +771,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -782,7 +812,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -807,7 +837,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -854,7 +884,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -885,7 +915,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{086FC864-88BE-4524-8C8E-D67D5CC31D33}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -920,7 +950,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8253E48-AC13-4C68-9E15-DF10E463748C}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -948,7 +978,68 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDAB02CB-AF8A-49D3-8080-6FFA51EF7AC4}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="29">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="29">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -991,68 +1082,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDAB02CB-AF8A-49D3-8080-6FFA51EF7AC4}">
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData>
-    <row r="1" spans="1:7" ht="29">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="29">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1101,7 +1131,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1126,7 +1156,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5C16204-518F-4A99-9E15-92D9161822C5}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1157,7 +1187,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1204,7 +1234,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16CA93A4-EF19-4F56-9442-DB07645E3971}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1251,7 +1281,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3C6F736-6B6A-4D47-9A3D-6735D564D2A8}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1298,7 +1328,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -1358,7 +1388,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{279E3CF8-6B58-482B-86D6-D534C8F178AB}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1393,7 +1423,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FBC1A4B-7999-43EC-A9B0-80154C608585}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1421,7 +1451,44 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6F5E429-4FED-4CBA-A7C3-3BB0B2C728FF}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="29">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="29">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1904BE75-2DA2-4667-82ED-527A58FD3287}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1449,33 +1516,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="10.7265625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EBEBA48-046F-4F91-8E90-E6AC9BDD1146}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1509,7 +1550,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F856F1BD-60DF-4B45-AA48-6580610D0108}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1563,7 +1604,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A2AE599-8749-4FEB-AADF-97800FD166F6}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -1629,7 +1670,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC885B18-8D7B-4141-98D3-4064592E6866}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -1693,7 +1734,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B4F42AD-06FB-4F9A-BDC5-0D988CFBC7C0}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1724,7 +1765,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DD0E29D-0CA1-467B-B75D-731ABD724820}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1755,7 +1796,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32378A89-E73B-434C-9031-5BC597A1049F}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1780,7 +1821,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01634569-4DCA-4114-8B9F-D11F9C8D6829}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1805,7 +1846,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32EC422E-61E5-4D5C-9000-57CFDB7C1C6E}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1835,6 +1876,32 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="10.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D22"/>
   <sheetViews>
@@ -2034,7 +2101,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9A9333D-303C-4846-B6A8-32400E420636}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -2076,7 +2143,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -2101,7 +2168,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -2130,7 +2197,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -2151,33 +2218,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
TC-82 added method added:getNewlyCreatedTestCaseId(),getLoggedInUserName(),verifyTestCaseCreationNotificationForNewTC() in AuthorTestCasePage.java  -> added data for TC-82
</commit_message>
<xml_diff>
--- a/testData/authorTestTabTestData/authorTestCaseTab_testData.xlsx
+++ b/testData/authorTestTabTestData/authorTestCaseTab_testData.xlsx
@@ -8,60 +8,61 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MohitAman\Desktop\UAT_NEXTNEXT_BLAZE_FRAMEWORK_AUTO\testData\authorTestTabTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B2085C3-4CA6-42FD-8A00-831AF77C1480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C4D13B-2C7B-4006-8258-42A02E803BAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddTest" sheetId="1" r:id="rId1"/>
     <sheet name="tc074" sheetId="40" r:id="rId2"/>
     <sheet name="tc075" sheetId="41" r:id="rId3"/>
     <sheet name="tc076" sheetId="42" r:id="rId4"/>
-    <sheet name="tc048" sheetId="2" r:id="rId5"/>
-    <sheet name="tc037" sheetId="3" r:id="rId6"/>
-    <sheet name="tc001" sheetId="4" r:id="rId7"/>
-    <sheet name="tc003" sheetId="5" r:id="rId8"/>
-    <sheet name="tc036" sheetId="6" r:id="rId9"/>
-    <sheet name="tc004" sheetId="7" r:id="rId10"/>
-    <sheet name="tc007" sheetId="8" r:id="rId11"/>
-    <sheet name="tc009" sheetId="9" r:id="rId12"/>
-    <sheet name="tc011" sheetId="10" r:id="rId13"/>
-    <sheet name="tc018" sheetId="11" r:id="rId14"/>
-    <sheet name="tc028" sheetId="12" r:id="rId15"/>
-    <sheet name="tc029" sheetId="13" r:id="rId16"/>
-    <sheet name="tc034" sheetId="14" r:id="rId17"/>
-    <sheet name="tc035" sheetId="15" r:id="rId18"/>
-    <sheet name="tc039" sheetId="16" r:id="rId19"/>
-    <sheet name="tc040" sheetId="17" r:id="rId20"/>
-    <sheet name="tc042" sheetId="18" r:id="rId21"/>
-    <sheet name="tc044" sheetId="19" r:id="rId22"/>
-    <sheet name="tc045" sheetId="20" r:id="rId23"/>
-    <sheet name="tc046" sheetId="21" r:id="rId24"/>
-    <sheet name="tc047" sheetId="22" r:id="rId25"/>
-    <sheet name="tc049" sheetId="23" r:id="rId26"/>
-    <sheet name="tc053" sheetId="24" r:id="rId27"/>
-    <sheet name="tc056" sheetId="25" r:id="rId28"/>
-    <sheet name="tc057" sheetId="26" r:id="rId29"/>
-    <sheet name="tc058" sheetId="27" r:id="rId30"/>
-    <sheet name="tc063" sheetId="28" r:id="rId31"/>
-    <sheet name="tc070" sheetId="29" r:id="rId32"/>
-    <sheet name="tc071" sheetId="30" r:id="rId33"/>
-    <sheet name="tc072" sheetId="31" r:id="rId34"/>
-    <sheet name="tc073" sheetId="32" r:id="rId35"/>
-    <sheet name="tc041" sheetId="33" r:id="rId36"/>
-    <sheet name="tc051" sheetId="34" r:id="rId37"/>
-    <sheet name="tc052" sheetId="35" r:id="rId38"/>
-    <sheet name="tc059" sheetId="36" r:id="rId39"/>
-    <sheet name="tc066" sheetId="37" r:id="rId40"/>
-    <sheet name="tc067" sheetId="38" r:id="rId41"/>
-    <sheet name="tc060" sheetId="39" r:id="rId42"/>
+    <sheet name="tc082" sheetId="43" r:id="rId5"/>
+    <sheet name="tc048" sheetId="2" r:id="rId6"/>
+    <sheet name="tc037" sheetId="3" r:id="rId7"/>
+    <sheet name="tc001" sheetId="4" r:id="rId8"/>
+    <sheet name="tc003" sheetId="5" r:id="rId9"/>
+    <sheet name="tc036" sheetId="6" r:id="rId10"/>
+    <sheet name="tc004" sheetId="7" r:id="rId11"/>
+    <sheet name="tc007" sheetId="8" r:id="rId12"/>
+    <sheet name="tc009" sheetId="9" r:id="rId13"/>
+    <sheet name="tc011" sheetId="10" r:id="rId14"/>
+    <sheet name="tc018" sheetId="11" r:id="rId15"/>
+    <sheet name="tc028" sheetId="12" r:id="rId16"/>
+    <sheet name="tc029" sheetId="13" r:id="rId17"/>
+    <sheet name="tc034" sheetId="14" r:id="rId18"/>
+    <sheet name="tc035" sheetId="15" r:id="rId19"/>
+    <sheet name="tc039" sheetId="16" r:id="rId20"/>
+    <sheet name="tc040" sheetId="17" r:id="rId21"/>
+    <sheet name="tc042" sheetId="18" r:id="rId22"/>
+    <sheet name="tc044" sheetId="19" r:id="rId23"/>
+    <sheet name="tc045" sheetId="20" r:id="rId24"/>
+    <sheet name="tc046" sheetId="21" r:id="rId25"/>
+    <sheet name="tc047" sheetId="22" r:id="rId26"/>
+    <sheet name="tc049" sheetId="23" r:id="rId27"/>
+    <sheet name="tc053" sheetId="24" r:id="rId28"/>
+    <sheet name="tc056" sheetId="25" r:id="rId29"/>
+    <sheet name="tc057" sheetId="26" r:id="rId30"/>
+    <sheet name="tc058" sheetId="27" r:id="rId31"/>
+    <sheet name="tc063" sheetId="28" r:id="rId32"/>
+    <sheet name="tc070" sheetId="29" r:id="rId33"/>
+    <sheet name="tc071" sheetId="30" r:id="rId34"/>
+    <sheet name="tc072" sheetId="31" r:id="rId35"/>
+    <sheet name="tc073" sheetId="32" r:id="rId36"/>
+    <sheet name="tc041" sheetId="33" r:id="rId37"/>
+    <sheet name="tc051" sheetId="34" r:id="rId38"/>
+    <sheet name="tc052" sheetId="35" r:id="rId39"/>
+    <sheet name="tc059" sheetId="36" r:id="rId40"/>
+    <sheet name="tc066" sheetId="37" r:id="rId41"/>
+    <sheet name="tc067" sheetId="38" r:id="rId42"/>
+    <sheet name="tc060" sheetId="39" r:id="rId43"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="83">
   <si>
     <t/>
   </si>
@@ -304,6 +305,12 @@
   </si>
   <si>
     <t>Prior</t>
+  </si>
+  <si>
+    <t>Creating testcase for automation TC-082</t>
+  </si>
+  <si>
+    <t>Testing Notification for create TC Jan 05-01-2026</t>
   </si>
 </sst>
 </file>
@@ -697,6 +704,41 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -719,7 +761,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -748,7 +790,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -771,7 +813,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -800,7 +842,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -835,7 +877,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -858,7 +900,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -881,7 +923,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -916,7 +958,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -932,47 +974,6 @@
     <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>31</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1039,6 +1040,47 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1067,7 +1109,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1096,7 +1138,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1119,7 +1161,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1160,7 +1202,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1207,7 +1249,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1230,7 +1272,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1259,7 +1301,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1300,7 +1342,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1334,53 +1376,6 @@
       </c>
       <c r="D2" t="s">
         <v>33</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1438,6 +1433,53 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -1490,7 +1532,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1519,7 +1561,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1542,7 +1584,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1565,7 +1607,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1594,7 +1636,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1641,7 +1683,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -1700,7 +1742,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -1759,7 +1801,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1781,35 +1823,6 @@
       </c>
       <c r="B2" t="s">
         <v>73</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1821,7 +1834,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3375FA57-6623-4363-8520-1724AAD516FA}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
@@ -1861,6 +1874,35 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1883,7 +1925,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1906,7 +1948,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2600-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1936,6 +1978,71 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9FA3E84-E8D4-4F66-ABFD-CBCCCFA9CB24}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="4" max="4" width="39.26953125" customWidth="1"/>
+    <col min="5" max="5" width="37.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -1994,7 +2101,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -2029,7 +2136,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -2052,7 +2159,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D22"/>
   <sheetViews>
@@ -2245,39 +2352,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
TC-83 added method added:verifyTestCaseUpdateNotification(String tcId),in AuthorTestCasePage.java  -> added data for TC-83
</commit_message>
<xml_diff>
--- a/testData/authorTestTabTestData/authorTestCaseTab_testData.xlsx
+++ b/testData/authorTestTabTestData/authorTestCaseTab_testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MohitAman\Desktop\UAT_NEXTNEXT_BLAZE_FRAMEWORK_AUTO\testData\authorTestTabTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C4D13B-2C7B-4006-8258-42A02E803BAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CE436E4-6F12-498E-B5A5-45304A0687A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddTest" sheetId="1" r:id="rId1"/>
@@ -18,51 +18,52 @@
     <sheet name="tc075" sheetId="41" r:id="rId3"/>
     <sheet name="tc076" sheetId="42" r:id="rId4"/>
     <sheet name="tc082" sheetId="43" r:id="rId5"/>
-    <sheet name="tc048" sheetId="2" r:id="rId6"/>
-    <sheet name="tc037" sheetId="3" r:id="rId7"/>
-    <sheet name="tc001" sheetId="4" r:id="rId8"/>
-    <sheet name="tc003" sheetId="5" r:id="rId9"/>
-    <sheet name="tc036" sheetId="6" r:id="rId10"/>
-    <sheet name="tc004" sheetId="7" r:id="rId11"/>
-    <sheet name="tc007" sheetId="8" r:id="rId12"/>
-    <sheet name="tc009" sheetId="9" r:id="rId13"/>
-    <sheet name="tc011" sheetId="10" r:id="rId14"/>
-    <sheet name="tc018" sheetId="11" r:id="rId15"/>
-    <sheet name="tc028" sheetId="12" r:id="rId16"/>
-    <sheet name="tc029" sheetId="13" r:id="rId17"/>
-    <sheet name="tc034" sheetId="14" r:id="rId18"/>
-    <sheet name="tc035" sheetId="15" r:id="rId19"/>
-    <sheet name="tc039" sheetId="16" r:id="rId20"/>
-    <sheet name="tc040" sheetId="17" r:id="rId21"/>
-    <sheet name="tc042" sheetId="18" r:id="rId22"/>
-    <sheet name="tc044" sheetId="19" r:id="rId23"/>
-    <sheet name="tc045" sheetId="20" r:id="rId24"/>
-    <sheet name="tc046" sheetId="21" r:id="rId25"/>
-    <sheet name="tc047" sheetId="22" r:id="rId26"/>
-    <sheet name="tc049" sheetId="23" r:id="rId27"/>
-    <sheet name="tc053" sheetId="24" r:id="rId28"/>
-    <sheet name="tc056" sheetId="25" r:id="rId29"/>
-    <sheet name="tc057" sheetId="26" r:id="rId30"/>
-    <sheet name="tc058" sheetId="27" r:id="rId31"/>
-    <sheet name="tc063" sheetId="28" r:id="rId32"/>
-    <sheet name="tc070" sheetId="29" r:id="rId33"/>
-    <sheet name="tc071" sheetId="30" r:id="rId34"/>
-    <sheet name="tc072" sheetId="31" r:id="rId35"/>
-    <sheet name="tc073" sheetId="32" r:id="rId36"/>
-    <sheet name="tc041" sheetId="33" r:id="rId37"/>
-    <sheet name="tc051" sheetId="34" r:id="rId38"/>
-    <sheet name="tc052" sheetId="35" r:id="rId39"/>
-    <sheet name="tc059" sheetId="36" r:id="rId40"/>
-    <sheet name="tc066" sheetId="37" r:id="rId41"/>
-    <sheet name="tc067" sheetId="38" r:id="rId42"/>
-    <sheet name="tc060" sheetId="39" r:id="rId43"/>
+    <sheet name="tc083" sheetId="44" r:id="rId6"/>
+    <sheet name="tc048" sheetId="2" r:id="rId7"/>
+    <sheet name="tc037" sheetId="3" r:id="rId8"/>
+    <sheet name="tc001" sheetId="4" r:id="rId9"/>
+    <sheet name="tc003" sheetId="5" r:id="rId10"/>
+    <sheet name="tc036" sheetId="6" r:id="rId11"/>
+    <sheet name="tc004" sheetId="7" r:id="rId12"/>
+    <sheet name="tc007" sheetId="8" r:id="rId13"/>
+    <sheet name="tc009" sheetId="9" r:id="rId14"/>
+    <sheet name="tc011" sheetId="10" r:id="rId15"/>
+    <sheet name="tc018" sheetId="11" r:id="rId16"/>
+    <sheet name="tc028" sheetId="12" r:id="rId17"/>
+    <sheet name="tc029" sheetId="13" r:id="rId18"/>
+    <sheet name="tc034" sheetId="14" r:id="rId19"/>
+    <sheet name="tc035" sheetId="15" r:id="rId20"/>
+    <sheet name="tc039" sheetId="16" r:id="rId21"/>
+    <sheet name="tc040" sheetId="17" r:id="rId22"/>
+    <sheet name="tc042" sheetId="18" r:id="rId23"/>
+    <sheet name="tc044" sheetId="19" r:id="rId24"/>
+    <sheet name="tc045" sheetId="20" r:id="rId25"/>
+    <sheet name="tc046" sheetId="21" r:id="rId26"/>
+    <sheet name="tc047" sheetId="22" r:id="rId27"/>
+    <sheet name="tc049" sheetId="23" r:id="rId28"/>
+    <sheet name="tc053" sheetId="24" r:id="rId29"/>
+    <sheet name="tc056" sheetId="25" r:id="rId30"/>
+    <sheet name="tc057" sheetId="26" r:id="rId31"/>
+    <sheet name="tc058" sheetId="27" r:id="rId32"/>
+    <sheet name="tc063" sheetId="28" r:id="rId33"/>
+    <sheet name="tc070" sheetId="29" r:id="rId34"/>
+    <sheet name="tc071" sheetId="30" r:id="rId35"/>
+    <sheet name="tc072" sheetId="31" r:id="rId36"/>
+    <sheet name="tc073" sheetId="32" r:id="rId37"/>
+    <sheet name="tc041" sheetId="33" r:id="rId38"/>
+    <sheet name="tc051" sheetId="34" r:id="rId39"/>
+    <sheet name="tc052" sheetId="35" r:id="rId40"/>
+    <sheet name="tc059" sheetId="36" r:id="rId41"/>
+    <sheet name="tc066" sheetId="37" r:id="rId42"/>
+    <sheet name="tc067" sheetId="38" r:id="rId43"/>
+    <sheet name="tc060" sheetId="39" r:id="rId44"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="84">
   <si>
     <t/>
   </si>
@@ -311,6 +312,9 @@
   </si>
   <si>
     <t>Testing Notification for create TC Jan 05-01-2026</t>
+  </si>
+  <si>
+    <t>Proir</t>
   </si>
 </sst>
 </file>
@@ -704,6 +708,201 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -738,7 +937,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -761,7 +960,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -790,7 +989,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -813,7 +1012,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -842,7 +1041,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -877,7 +1076,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -900,7 +1099,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -923,7 +1122,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -951,29 +1150,6 @@
       </c>
       <c r="C2" t="s">
         <v>21</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1040,6 +1216,29 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1080,7 +1279,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1109,7 +1308,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1138,7 +1337,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1161,7 +1360,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1202,7 +1401,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1249,7 +1448,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1272,7 +1471,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1301,7 +1500,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1335,47 +1534,6 @@
       </c>
       <c r="D2" t="s">
         <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1433,6 +1591,47 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1479,7 +1678,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -1532,7 +1731,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1561,7 +1760,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1584,7 +1783,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1607,7 +1806,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1636,7 +1835,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1683,7 +1882,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -1742,7 +1941,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -1794,35 +1993,6 @@
       </c>
       <c r="G2" t="s">
         <v>71</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" t="s">
-        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1874,6 +2044,35 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1902,7 +2101,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1925,7 +2124,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1948,7 +2147,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2600-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1981,7 +2180,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9FA3E84-E8D4-4F66-ABFD-CBCCCFA9CB24}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:G2"/>
     </sheetView>
   </sheetViews>
@@ -2043,6 +2242,76 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A81839A3-FAE3-4F46-B003-D7D669BBB1E5}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="7" max="7" width="12.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -2101,7 +2370,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -2136,7 +2405,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -2157,199 +2426,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:D22"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B15" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B19" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" t="s">
-        <v>0</v>
-      </c>
-      <c r="B22" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
TC-84 added method added:verifyTestCaseApproveNotification(String tcId),in AuthorTestCasePage.java  -> added data for TC-84
</commit_message>
<xml_diff>
--- a/testData/authorTestTabTestData/authorTestCaseTab_testData.xlsx
+++ b/testData/authorTestTabTestData/authorTestCaseTab_testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MohitAman\Desktop\UAT_NEXTNEXT_BLAZE_FRAMEWORK_AUTO\testData\authorTestTabTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CE436E4-6F12-498E-B5A5-45304A0687A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2CEE369-0978-489B-94DC-DDC084C5C64C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddTest" sheetId="1" r:id="rId1"/>
@@ -19,51 +19,52 @@
     <sheet name="tc076" sheetId="42" r:id="rId4"/>
     <sheet name="tc082" sheetId="43" r:id="rId5"/>
     <sheet name="tc083" sheetId="44" r:id="rId6"/>
-    <sheet name="tc048" sheetId="2" r:id="rId7"/>
-    <sheet name="tc037" sheetId="3" r:id="rId8"/>
-    <sheet name="tc001" sheetId="4" r:id="rId9"/>
-    <sheet name="tc003" sheetId="5" r:id="rId10"/>
-    <sheet name="tc036" sheetId="6" r:id="rId11"/>
-    <sheet name="tc004" sheetId="7" r:id="rId12"/>
-    <sheet name="tc007" sheetId="8" r:id="rId13"/>
-    <sheet name="tc009" sheetId="9" r:id="rId14"/>
-    <sheet name="tc011" sheetId="10" r:id="rId15"/>
-    <sheet name="tc018" sheetId="11" r:id="rId16"/>
-    <sheet name="tc028" sheetId="12" r:id="rId17"/>
-    <sheet name="tc029" sheetId="13" r:id="rId18"/>
-    <sheet name="tc034" sheetId="14" r:id="rId19"/>
-    <sheet name="tc035" sheetId="15" r:id="rId20"/>
-    <sheet name="tc039" sheetId="16" r:id="rId21"/>
-    <sheet name="tc040" sheetId="17" r:id="rId22"/>
-    <sheet name="tc042" sheetId="18" r:id="rId23"/>
-    <sheet name="tc044" sheetId="19" r:id="rId24"/>
-    <sheet name="tc045" sheetId="20" r:id="rId25"/>
-    <sheet name="tc046" sheetId="21" r:id="rId26"/>
-    <sheet name="tc047" sheetId="22" r:id="rId27"/>
-    <sheet name="tc049" sheetId="23" r:id="rId28"/>
-    <sheet name="tc053" sheetId="24" r:id="rId29"/>
-    <sheet name="tc056" sheetId="25" r:id="rId30"/>
-    <sheet name="tc057" sheetId="26" r:id="rId31"/>
-    <sheet name="tc058" sheetId="27" r:id="rId32"/>
-    <sheet name="tc063" sheetId="28" r:id="rId33"/>
-    <sheet name="tc070" sheetId="29" r:id="rId34"/>
-    <sheet name="tc071" sheetId="30" r:id="rId35"/>
-    <sheet name="tc072" sheetId="31" r:id="rId36"/>
-    <sheet name="tc073" sheetId="32" r:id="rId37"/>
-    <sheet name="tc041" sheetId="33" r:id="rId38"/>
-    <sheet name="tc051" sheetId="34" r:id="rId39"/>
-    <sheet name="tc052" sheetId="35" r:id="rId40"/>
-    <sheet name="tc059" sheetId="36" r:id="rId41"/>
-    <sheet name="tc066" sheetId="37" r:id="rId42"/>
-    <sheet name="tc067" sheetId="38" r:id="rId43"/>
-    <sheet name="tc060" sheetId="39" r:id="rId44"/>
+    <sheet name="tc084" sheetId="45" r:id="rId7"/>
+    <sheet name="tc048" sheetId="2" r:id="rId8"/>
+    <sheet name="tc037" sheetId="3" r:id="rId9"/>
+    <sheet name="tc001" sheetId="4" r:id="rId10"/>
+    <sheet name="tc003" sheetId="5" r:id="rId11"/>
+    <sheet name="tc036" sheetId="6" r:id="rId12"/>
+    <sheet name="tc004" sheetId="7" r:id="rId13"/>
+    <sheet name="tc007" sheetId="8" r:id="rId14"/>
+    <sheet name="tc009" sheetId="9" r:id="rId15"/>
+    <sheet name="tc011" sheetId="10" r:id="rId16"/>
+    <sheet name="tc018" sheetId="11" r:id="rId17"/>
+    <sheet name="tc028" sheetId="12" r:id="rId18"/>
+    <sheet name="tc029" sheetId="13" r:id="rId19"/>
+    <sheet name="tc034" sheetId="14" r:id="rId20"/>
+    <sheet name="tc035" sheetId="15" r:id="rId21"/>
+    <sheet name="tc039" sheetId="16" r:id="rId22"/>
+    <sheet name="tc040" sheetId="17" r:id="rId23"/>
+    <sheet name="tc042" sheetId="18" r:id="rId24"/>
+    <sheet name="tc044" sheetId="19" r:id="rId25"/>
+    <sheet name="tc045" sheetId="20" r:id="rId26"/>
+    <sheet name="tc046" sheetId="21" r:id="rId27"/>
+    <sheet name="tc047" sheetId="22" r:id="rId28"/>
+    <sheet name="tc049" sheetId="23" r:id="rId29"/>
+    <sheet name="tc053" sheetId="24" r:id="rId30"/>
+    <sheet name="tc056" sheetId="25" r:id="rId31"/>
+    <sheet name="tc057" sheetId="26" r:id="rId32"/>
+    <sheet name="tc058" sheetId="27" r:id="rId33"/>
+    <sheet name="tc063" sheetId="28" r:id="rId34"/>
+    <sheet name="tc070" sheetId="29" r:id="rId35"/>
+    <sheet name="tc071" sheetId="30" r:id="rId36"/>
+    <sheet name="tc072" sheetId="31" r:id="rId37"/>
+    <sheet name="tc073" sheetId="32" r:id="rId38"/>
+    <sheet name="tc041" sheetId="33" r:id="rId39"/>
+    <sheet name="tc051" sheetId="34" r:id="rId40"/>
+    <sheet name="tc052" sheetId="35" r:id="rId41"/>
+    <sheet name="tc059" sheetId="36" r:id="rId42"/>
+    <sheet name="tc066" sheetId="37" r:id="rId43"/>
+    <sheet name="tc067" sheetId="38" r:id="rId44"/>
+    <sheet name="tc060" sheetId="39" r:id="rId45"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="84">
   <si>
     <t/>
   </si>
@@ -708,6 +709,29 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D22"/>
   <sheetViews>
@@ -902,7 +926,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -937,7 +961,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -960,7 +984,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -989,7 +1013,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1012,7 +1036,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1041,7 +1065,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -1076,7 +1100,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1099,7 +1123,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1115,41 +1139,6 @@
     <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1216,6 +1205,41 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1238,7 +1262,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1279,7 +1303,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1308,7 +1332,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1337,7 +1361,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1360,7 +1384,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1401,7 +1425,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1448,7 +1472,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1471,7 +1495,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1493,47 +1517,6 @@
       </c>
       <c r="B2" t="s">
         <v>45</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1591,6 +1574,47 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1631,7 +1655,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1678,7 +1702,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -1731,7 +1755,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1760,7 +1784,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1783,7 +1807,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1806,7 +1830,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1835,7 +1859,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1882,67 +1906,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2044,6 +2009,65 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -2072,7 +2096,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -2101,7 +2125,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -2124,7 +2148,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -2147,7 +2171,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2600-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -2245,8 +2269,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A81839A3-FAE3-4F46-B003-D7D669BBB1E5}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2312,6 +2336,73 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{793D6349-D811-4E58-A638-D18DC4A64140}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -2370,7 +2461,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -2403,27 +2494,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
TC-85 added method added:verifyTestRunCreatedNotification(String tcId),in AuthorTestCasePage.java  -> added data for TC-85
</commit_message>
<xml_diff>
--- a/testData/authorTestTabTestData/authorTestCaseTab_testData.xlsx
+++ b/testData/authorTestTabTestData/authorTestCaseTab_testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MohitAman\Desktop\UAT_NEXTNEXT_BLAZE_FRAMEWORK_AUTO\testData\authorTestTabTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE7D48E4-3E7E-4BCA-91C9-3C01BC22D93D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F637CBFC-FF0B-44C1-ABA7-73D1FF865E13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddTest" sheetId="1" r:id="rId1"/>
@@ -20,51 +20,52 @@
     <sheet name="tc082" sheetId="43" r:id="rId5"/>
     <sheet name="tc083" sheetId="44" r:id="rId6"/>
     <sheet name="tc084" sheetId="45" r:id="rId7"/>
-    <sheet name="tc048" sheetId="2" r:id="rId8"/>
-    <sheet name="tc037" sheetId="3" r:id="rId9"/>
-    <sheet name="tc001" sheetId="4" r:id="rId10"/>
-    <sheet name="tc003" sheetId="5" r:id="rId11"/>
-    <sheet name="tc036" sheetId="6" r:id="rId12"/>
-    <sheet name="tc004" sheetId="7" r:id="rId13"/>
-    <sheet name="tc007" sheetId="8" r:id="rId14"/>
-    <sheet name="tc009" sheetId="9" r:id="rId15"/>
-    <sheet name="tc011" sheetId="10" r:id="rId16"/>
-    <sheet name="tc018" sheetId="11" r:id="rId17"/>
-    <sheet name="tc028" sheetId="12" r:id="rId18"/>
-    <sheet name="tc029" sheetId="13" r:id="rId19"/>
-    <sheet name="tc034" sheetId="14" r:id="rId20"/>
-    <sheet name="tc035" sheetId="15" r:id="rId21"/>
-    <sheet name="tc039" sheetId="16" r:id="rId22"/>
-    <sheet name="tc040" sheetId="17" r:id="rId23"/>
-    <sheet name="tc042" sheetId="18" r:id="rId24"/>
-    <sheet name="tc044" sheetId="19" r:id="rId25"/>
-    <sheet name="tc045" sheetId="20" r:id="rId26"/>
-    <sheet name="tc046" sheetId="21" r:id="rId27"/>
-    <sheet name="tc047" sheetId="22" r:id="rId28"/>
-    <sheet name="tc049" sheetId="23" r:id="rId29"/>
-    <sheet name="tc053" sheetId="24" r:id="rId30"/>
-    <sheet name="tc056" sheetId="25" r:id="rId31"/>
-    <sheet name="tc057" sheetId="26" r:id="rId32"/>
-    <sheet name="tc058" sheetId="27" r:id="rId33"/>
-    <sheet name="tc063" sheetId="28" r:id="rId34"/>
-    <sheet name="tc070" sheetId="29" r:id="rId35"/>
-    <sheet name="tc071" sheetId="30" r:id="rId36"/>
-    <sheet name="tc072" sheetId="31" r:id="rId37"/>
-    <sheet name="tc073" sheetId="32" r:id="rId38"/>
-    <sheet name="tc041" sheetId="33" r:id="rId39"/>
-    <sheet name="tc051" sheetId="34" r:id="rId40"/>
-    <sheet name="tc052" sheetId="35" r:id="rId41"/>
-    <sheet name="tc059" sheetId="36" r:id="rId42"/>
-    <sheet name="tc066" sheetId="37" r:id="rId43"/>
-    <sheet name="tc067" sheetId="38" r:id="rId44"/>
-    <sheet name="tc060" sheetId="39" r:id="rId45"/>
+    <sheet name="tc085" sheetId="46" r:id="rId8"/>
+    <sheet name="tc048" sheetId="2" r:id="rId9"/>
+    <sheet name="tc037" sheetId="3" r:id="rId10"/>
+    <sheet name="tc001" sheetId="4" r:id="rId11"/>
+    <sheet name="tc003" sheetId="5" r:id="rId12"/>
+    <sheet name="tc036" sheetId="6" r:id="rId13"/>
+    <sheet name="tc004" sheetId="7" r:id="rId14"/>
+    <sheet name="tc007" sheetId="8" r:id="rId15"/>
+    <sheet name="tc009" sheetId="9" r:id="rId16"/>
+    <sheet name="tc011" sheetId="10" r:id="rId17"/>
+    <sheet name="tc018" sheetId="11" r:id="rId18"/>
+    <sheet name="tc028" sheetId="12" r:id="rId19"/>
+    <sheet name="tc029" sheetId="13" r:id="rId20"/>
+    <sheet name="tc034" sheetId="14" r:id="rId21"/>
+    <sheet name="tc035" sheetId="15" r:id="rId22"/>
+    <sheet name="tc039" sheetId="16" r:id="rId23"/>
+    <sheet name="tc040" sheetId="17" r:id="rId24"/>
+    <sheet name="tc042" sheetId="18" r:id="rId25"/>
+    <sheet name="tc044" sheetId="19" r:id="rId26"/>
+    <sheet name="tc045" sheetId="20" r:id="rId27"/>
+    <sheet name="tc046" sheetId="21" r:id="rId28"/>
+    <sheet name="tc047" sheetId="22" r:id="rId29"/>
+    <sheet name="tc049" sheetId="23" r:id="rId30"/>
+    <sheet name="tc053" sheetId="24" r:id="rId31"/>
+    <sheet name="tc056" sheetId="25" r:id="rId32"/>
+    <sheet name="tc057" sheetId="26" r:id="rId33"/>
+    <sheet name="tc058" sheetId="27" r:id="rId34"/>
+    <sheet name="tc063" sheetId="28" r:id="rId35"/>
+    <sheet name="tc070" sheetId="29" r:id="rId36"/>
+    <sheet name="tc071" sheetId="30" r:id="rId37"/>
+    <sheet name="tc072" sheetId="31" r:id="rId38"/>
+    <sheet name="tc073" sheetId="32" r:id="rId39"/>
+    <sheet name="tc041" sheetId="33" r:id="rId40"/>
+    <sheet name="tc051" sheetId="34" r:id="rId41"/>
+    <sheet name="tc052" sheetId="35" r:id="rId42"/>
+    <sheet name="tc059" sheetId="36" r:id="rId43"/>
+    <sheet name="tc066" sheetId="37" r:id="rId44"/>
+    <sheet name="tc067" sheetId="38" r:id="rId45"/>
+    <sheet name="tc060" sheetId="39" r:id="rId46"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="86">
   <si>
     <t/>
   </si>
@@ -316,6 +317,12 @@
   </si>
   <si>
     <t>Proir</t>
+  </si>
+  <si>
+    <t>release</t>
+  </si>
+  <si>
+    <t>Release 06-01-2025</t>
   </si>
 </sst>
 </file>
@@ -709,6 +716,41 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -731,7 +773,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D22"/>
   <sheetViews>
@@ -926,7 +968,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -961,7 +1003,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -984,7 +1026,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1013,7 +1055,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1036,7 +1078,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1065,7 +1107,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -1100,7 +1142,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1116,29 +1158,6 @@
     <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>25</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1205,6 +1224,29 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -1239,7 +1281,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1262,7 +1304,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1303,7 +1345,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1332,7 +1374,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1361,7 +1403,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1384,7 +1426,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1425,7 +1467,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1472,7 +1514,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1488,35 +1530,6 @@
     <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>31</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1574,6 +1587,35 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1614,7 +1656,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1655,7 +1697,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1702,7 +1744,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -1755,7 +1797,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1784,7 +1826,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1807,7 +1849,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1830,7 +1872,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1859,7 +1901,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1899,65 +1941,6 @@
       </c>
       <c r="E2" t="s">
         <v>60</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G2" t="s">
-        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -2009,6 +1992,65 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -2067,7 +2109,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -2096,7 +2138,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -2125,7 +2167,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -2148,7 +2190,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -2171,7 +2213,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2600-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -2339,8 +2381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{793D6349-D811-4E58-A638-D18DC4A64140}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2403,6 +2445,76 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4420E51E-4F62-4C37-8E5A-01D5B5A5FEF6}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="7" max="7" width="11.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -2459,39 +2571,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
TC-79 updated added method isApproveButtonDisabled() in IndividualTestCasePage.java
</commit_message>
<xml_diff>
--- a/testData/authorTestTabTestData/authorTestCaseTab_testData.xlsx
+++ b/testData/authorTestTabTestData/authorTestCaseTab_testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MohitAman\Desktop\UAT_NEXTNEXT_BLAZE_FRAMEWORK_AUTO\testData\authorTestTabTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAB5003C-B093-436B-88DB-357FD0671F22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD530AF-38B6-44F3-B78C-0F45B86668E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="20" activeTab="24" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="32" activeTab="39" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddTest" sheetId="1" r:id="rId1"/>
@@ -52,20 +52,21 @@
     <sheet name="tc071" sheetId="30" r:id="rId37"/>
     <sheet name="tc072" sheetId="31" r:id="rId38"/>
     <sheet name="tc073" sheetId="32" r:id="rId39"/>
-    <sheet name="tc041" sheetId="33" r:id="rId40"/>
-    <sheet name="tc051" sheetId="34" r:id="rId41"/>
-    <sheet name="tc052" sheetId="35" r:id="rId42"/>
-    <sheet name="tc059" sheetId="36" r:id="rId43"/>
-    <sheet name="tc066" sheetId="37" r:id="rId44"/>
-    <sheet name="tc067" sheetId="38" r:id="rId45"/>
-    <sheet name="tc060" sheetId="39" r:id="rId46"/>
+    <sheet name="tc079" sheetId="47" r:id="rId40"/>
+    <sheet name="tc041" sheetId="33" r:id="rId41"/>
+    <sheet name="tc051" sheetId="34" r:id="rId42"/>
+    <sheet name="tc052" sheetId="35" r:id="rId43"/>
+    <sheet name="tc059" sheetId="36" r:id="rId44"/>
+    <sheet name="tc066" sheetId="37" r:id="rId45"/>
+    <sheet name="tc067" sheetId="38" r:id="rId46"/>
+    <sheet name="tc060" sheetId="39" r:id="rId47"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="86">
   <si>
     <t/>
   </si>
@@ -1378,7 +1379,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
@@ -1660,7 +1661,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
@@ -1992,6 +1995,49 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F56B1014-60C3-4138-A1B0-297C0E0F4CA2}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -2050,7 +2096,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -2109,7 +2155,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -2138,7 +2184,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -2167,7 +2213,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -2190,7 +2236,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -2213,7 +2259,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2600-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>

</xml_diff>

<commit_message>
Corrected TC-12 added data and also changed locator getAllFeatures()
</commit_message>
<xml_diff>
--- a/testData/authorTestTabTestData/authorTestCaseTab_testData.xlsx
+++ b/testData/authorTestTabTestData/authorTestCaseTab_testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MohitAman\Desktop\UAT_NEXTNEXT_BLAZE_FRAMEWORK_AUTO\testData\authorTestTabTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0E36E87-B327-40CE-AA61-98DD0D75F75C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95132E4A-2401-4DDF-82E6-91E8056BE3A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="31" activeTab="39" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="10" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddTest" sheetId="1" r:id="rId1"/>
@@ -30,43 +30,44 @@
     <sheet name="tc007" sheetId="8" r:id="rId15"/>
     <sheet name="tc009" sheetId="9" r:id="rId16"/>
     <sheet name="tc011" sheetId="10" r:id="rId17"/>
-    <sheet name="tc018" sheetId="11" r:id="rId18"/>
-    <sheet name="tc028" sheetId="12" r:id="rId19"/>
-    <sheet name="tc029" sheetId="13" r:id="rId20"/>
-    <sheet name="tc034" sheetId="14" r:id="rId21"/>
-    <sheet name="tc035" sheetId="15" r:id="rId22"/>
-    <sheet name="tc039" sheetId="16" r:id="rId23"/>
-    <sheet name="tc040" sheetId="17" r:id="rId24"/>
-    <sheet name="tc042" sheetId="18" r:id="rId25"/>
-    <sheet name="tc044" sheetId="19" r:id="rId26"/>
-    <sheet name="tc045" sheetId="20" r:id="rId27"/>
-    <sheet name="tc046" sheetId="21" r:id="rId28"/>
-    <sheet name="tc047" sheetId="22" r:id="rId29"/>
-    <sheet name="tc049" sheetId="23" r:id="rId30"/>
-    <sheet name="tc053" sheetId="24" r:id="rId31"/>
-    <sheet name="tc056" sheetId="25" r:id="rId32"/>
-    <sheet name="tc057" sheetId="26" r:id="rId33"/>
-    <sheet name="tc058" sheetId="27" r:id="rId34"/>
-    <sheet name="tc063" sheetId="28" r:id="rId35"/>
-    <sheet name="tc070" sheetId="29" r:id="rId36"/>
-    <sheet name="tc071" sheetId="30" r:id="rId37"/>
-    <sheet name="tc072" sheetId="31" r:id="rId38"/>
-    <sheet name="tc073" sheetId="32" r:id="rId39"/>
-    <sheet name="tc079" sheetId="47" r:id="rId40"/>
-    <sheet name="tc041" sheetId="33" r:id="rId41"/>
-    <sheet name="tc051" sheetId="34" r:id="rId42"/>
-    <sheet name="tc052" sheetId="35" r:id="rId43"/>
-    <sheet name="tc059" sheetId="36" r:id="rId44"/>
-    <sheet name="tc066" sheetId="37" r:id="rId45"/>
-    <sheet name="tc067" sheetId="38" r:id="rId46"/>
-    <sheet name="tc060" sheetId="39" r:id="rId47"/>
+    <sheet name="tc012" sheetId="49" r:id="rId18"/>
+    <sheet name="tc018" sheetId="11" r:id="rId19"/>
+    <sheet name="tc028" sheetId="12" r:id="rId20"/>
+    <sheet name="tc029" sheetId="13" r:id="rId21"/>
+    <sheet name="tc034" sheetId="14" r:id="rId22"/>
+    <sheet name="tc035" sheetId="15" r:id="rId23"/>
+    <sheet name="tc039" sheetId="16" r:id="rId24"/>
+    <sheet name="tc040" sheetId="17" r:id="rId25"/>
+    <sheet name="tc042" sheetId="18" r:id="rId26"/>
+    <sheet name="tc044" sheetId="19" r:id="rId27"/>
+    <sheet name="tc045" sheetId="20" r:id="rId28"/>
+    <sheet name="tc046" sheetId="21" r:id="rId29"/>
+    <sheet name="tc047" sheetId="22" r:id="rId30"/>
+    <sheet name="tc049" sheetId="23" r:id="rId31"/>
+    <sheet name="tc053" sheetId="24" r:id="rId32"/>
+    <sheet name="tc056" sheetId="25" r:id="rId33"/>
+    <sheet name="tc057" sheetId="26" r:id="rId34"/>
+    <sheet name="tc058" sheetId="27" r:id="rId35"/>
+    <sheet name="tc063" sheetId="28" r:id="rId36"/>
+    <sheet name="tc070" sheetId="29" r:id="rId37"/>
+    <sheet name="tc071" sheetId="30" r:id="rId38"/>
+    <sheet name="tc072" sheetId="31" r:id="rId39"/>
+    <sheet name="tc073" sheetId="32" r:id="rId40"/>
+    <sheet name="tc079" sheetId="47" r:id="rId41"/>
+    <sheet name="tc041" sheetId="33" r:id="rId42"/>
+    <sheet name="tc051" sheetId="34" r:id="rId43"/>
+    <sheet name="tc052" sheetId="35" r:id="rId44"/>
+    <sheet name="tc059" sheetId="36" r:id="rId45"/>
+    <sheet name="tc066" sheetId="37" r:id="rId46"/>
+    <sheet name="tc067" sheetId="38" r:id="rId47"/>
+    <sheet name="tc060" sheetId="39" r:id="rId48"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="86">
   <si>
     <t/>
   </si>
@@ -757,7 +758,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
@@ -1012,7 +1015,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
@@ -1087,7 +1092,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
@@ -1113,6 +1120,34 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80738B24-AA6E-4279-9600-2A504CCA6F33}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="14.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -1140,29 +1175,6 @@
       </c>
       <c r="C2" t="s">
         <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1229,6 +1241,29 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1251,7 +1286,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -1286,7 +1321,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1311,7 +1346,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1352,7 +1387,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1381,7 +1416,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1410,7 +1445,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1433,7 +1468,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1474,7 +1509,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1514,29 +1549,6 @@
       </c>
       <c r="E2" t="s">
         <v>14</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1594,6 +1606,29 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1622,7 +1657,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1663,7 +1698,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1706,7 +1741,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1753,7 +1788,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -1806,7 +1841,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1835,7 +1870,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1858,7 +1893,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1881,7 +1916,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1903,53 +1938,6 @@
       </c>
       <c r="B2" t="s">
         <v>59</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E2" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -2001,10 +1989,57 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F56B1014-60C3-4138-A1B0-297C0E0F4CA2}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
@@ -2043,7 +2078,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -2102,7 +2137,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -2161,7 +2196,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -2190,7 +2225,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -2219,7 +2254,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -2242,7 +2277,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -2265,7 +2300,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2600-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>

</xml_diff>